<commit_message>
Update Status Google Sheet
</commit_message>
<xml_diff>
--- a/Bot1/Config.xlsx
+++ b/Bot1/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\UiPath\bot1\Bot1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/29f27606214cd687/Documents/UiPath/BOT1(new)/Bot1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76919E00-8C62-4E5C-AEA5-C98D2790DA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{76919E00-8C62-4E5C-AEA5-C98D2790DA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24E063FF-649C-43F8-B969-CDD1D7A8BD15}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{05E979CD-2C89-4B74-8A78-07879031F12A}"/>
   </bookViews>
@@ -54,10 +54,10 @@
     <t>Subject</t>
   </si>
   <si>
-    <t>From excel - New Employe Boarding Annoucement September 2023</t>
-  </si>
-  <si>
     <t>zeerx7@gmail.com,Leader; pausi347@gmail.com,HC Team; rosadirully5@gmail.com,Leader</t>
+  </si>
+  <si>
+    <t>New Employe Boarding Annoucement September 2023</t>
   </si>
 </sst>
 </file>
@@ -128,14 +128,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -173,7 +169,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -279,7 +275,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -421,7 +417,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -432,7 +428,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -469,7 +465,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>